<commit_message>
version 2.0.0 upgrade ftest
</commit_message>
<xml_diff>
--- a/ftest/data/fm3/Worked_example_policy_calculation_1.xlsx
+++ b/ftest/data/fm3/Worked_example_policy_calculation_1.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\2 Working Parties\Financial Module\Worked examples for public\01 Final\Worked_example_policy_calculation_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\data\fm3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18960" windowHeight="8655"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18960" windowHeight="8652"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="13" r:id="rId1"/>
     <sheet name="Policy Calculation" sheetId="11" r:id="rId2"/>
     <sheet name="Oasis Implementation" sheetId="12" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="135">
   <si>
     <t>Limit</t>
   </si>
@@ -272,37 +272,13 @@
     <t>Oasis Data tables</t>
   </si>
   <si>
-    <t>AGG_ID</t>
-  </si>
-  <si>
     <t>PolicyTC</t>
   </si>
   <si>
-    <t>LAYER_ID</t>
-  </si>
-  <si>
-    <t>POLICYTC_ID</t>
-  </si>
-  <si>
-    <t>AREAPERIL_ID</t>
-  </si>
-  <si>
-    <t>VULNERABILITY_ID</t>
-  </si>
-  <si>
-    <t>TIV</t>
-  </si>
-  <si>
     <t>IL = Sum(S2)</t>
   </si>
   <si>
     <t>GUL = V * DR</t>
-  </si>
-  <si>
-    <t>Exposure item file</t>
-  </si>
-  <si>
-    <t>GROUP_ID</t>
   </si>
   <si>
     <t>Exposures</t>
@@ -527,49 +503,85 @@
     <t>Made-up example of a residential insurance policy;</t>
   </si>
   <si>
-    <t>LEVEL_ID</t>
-  </si>
-  <si>
-    <t>CALCRULE_ID</t>
-  </si>
-  <si>
-    <t>ALLOCRULE_ID</t>
-  </si>
-  <si>
-    <t>SOURCERULE_ID</t>
-  </si>
-  <si>
-    <t>LEVELRULE_ID</t>
-  </si>
-  <si>
-    <t>DED</t>
-  </si>
-  <si>
-    <t>LIM</t>
-  </si>
-  <si>
-    <t>SHARE_PROP_OF_LIM</t>
-  </si>
-  <si>
-    <t>DEDUCTIBLE_PROP_OF_LOSS</t>
-  </si>
-  <si>
-    <t>LIMIT_PROP_OF_LOSS</t>
-  </si>
-  <si>
-    <t>DEDUCTIBLE_PROP_OF_TIV</t>
-  </si>
-  <si>
-    <t>LIMIT_PROP_OF_TIV</t>
-  </si>
-  <si>
-    <t>DEDUCTIBLE_PROP_OF_LIMIT</t>
+    <t>Item file</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>coverage_id</t>
+  </si>
+  <si>
+    <t>areaperil_id</t>
+  </si>
+  <si>
+    <t>vulnerability_id</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>tiv</t>
+  </si>
+  <si>
+    <t>Coverage file</t>
+  </si>
+  <si>
+    <t>from_agg_id</t>
+  </si>
+  <si>
+    <t>level_id</t>
+  </si>
+  <si>
+    <t>to_agg_id</t>
+  </si>
+  <si>
+    <t>layer_id</t>
+  </si>
+  <si>
+    <t>agg_id</t>
+  </si>
+  <si>
+    <t>policytc_id</t>
+  </si>
+  <si>
+    <t>calcrule_id</t>
+  </si>
+  <si>
+    <t>allocrule_id</t>
+  </si>
+  <si>
+    <t>ccy_id</t>
+  </si>
+  <si>
+    <t>deductible</t>
+  </si>
+  <si>
+    <t>limits</t>
+  </si>
+  <si>
+    <t>share_prop_of_lim</t>
+  </si>
+  <si>
+    <t>deductible_prop_of_loss</t>
+  </si>
+  <si>
+    <t>limit_prop_of_loss</t>
+  </si>
+  <si>
+    <t>deductible_prop_of_tiv</t>
+  </si>
+  <si>
+    <t>limit_prop_of_tiv</t>
+  </si>
+  <si>
+    <t>deductible_prop_of_limit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1044,6 +1056,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1079,6 +1108,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1259,121 +1305,121 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="55" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="55" t="s">
+    <row r="21" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="55" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="55" t="s">
-        <v>111</v>
-      </c>
       <c r="Q21" s="25"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="55" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="55" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="55" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="56" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1397,50 +1443,50 @@
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1510,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -1472,7 +1518,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1480,7 +1526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -1496,7 +1542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1504,7 +1550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1512,72 +1558,72 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1595,7 +1641,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="10"/>
@@ -1611,7 +1657,7 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="39"/>
       <c r="B35" s="40"/>
       <c r="C35" s="41" t="s">
@@ -1629,7 +1675,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="51" t="s">
         <v>38</v>
       </c>
@@ -1652,7 +1698,7 @@
       <c r="H36" s="44"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="45" t="s">
         <v>6</v>
       </c>
@@ -1664,7 +1710,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="44"/>
     </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="45" t="s">
         <v>26</v>
       </c>
@@ -1686,12 +1732,12 @@
       <c r="G38" s="7"/>
       <c r="H38" s="44"/>
     </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="46" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -1700,7 +1746,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="44"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="45" t="s">
         <v>1</v>
       </c>
@@ -1722,7 +1768,7 @@
       <c r="G40" s="7"/>
       <c r="H40" s="44"/>
     </row>
-    <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="45" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1790,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="44"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="45"/>
       <c r="B42" s="7"/>
       <c r="C42" s="11"/>
@@ -1754,7 +1800,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="44"/>
     </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="51" t="s">
         <v>44</v>
       </c>
@@ -1766,7 +1812,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="44"/>
     </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="45" t="s">
         <v>35</v>
       </c>
@@ -1788,7 +1834,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="44"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="45"/>
       <c r="B45" s="7"/>
       <c r="C45" s="11"/>
@@ -1798,7 +1844,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="44"/>
     </row>
-    <row r="46" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
         <v>36</v>
       </c>
@@ -1812,12 +1858,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="45" t="s">
         <v>37</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C47" s="13">
         <f>C44*C38</f>
@@ -1838,12 +1884,12 @@
       <c r="G47" s="7"/>
       <c r="H47" s="44"/>
     </row>
-    <row r="48" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C48" s="13">
         <f>MAX(C47-C40,0)</f>
@@ -1864,12 +1910,12 @@
       <c r="G48" s="7"/>
       <c r="H48" s="44"/>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C49" s="13">
         <f>MIN(C48,C41)</f>
@@ -1890,12 +1936,12 @@
       <c r="G49" s="7"/>
       <c r="H49" s="44"/>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="47" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C50" s="49"/>
       <c r="D50" s="49"/>
@@ -1922,42 +1968,44 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>58</v>
       </c>
@@ -1974,7 +2022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>77</v>
       </c>
@@ -1991,17 +2039,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
       <c r="B6" s="31"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B7" s="34"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>65</v>
       </c>
@@ -2009,7 +2057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>66</v>
       </c>
@@ -2017,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>67</v>
       </c>
@@ -2025,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>1</v>
       </c>
@@ -2033,7 +2081,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>0</v>
       </c>
@@ -2041,20 +2089,20 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>76</v>
       </c>
@@ -2062,10 +2110,13 @@
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="K17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
         <v>70</v>
       </c>
@@ -2075,22 +2126,28 @@
       <c r="C18" s="37"/>
       <c r="D18" s="26"/>
       <c r="E18" s="35" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>1</v>
       </c>
@@ -2108,13 +2165,19 @@
         <v>1</v>
       </c>
       <c r="H19" s="19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="19">
         <v>1000000</v>
       </c>
-      <c r="I19" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>2</v>
       </c>
@@ -2129,16 +2192,22 @@
         <v>1</v>
       </c>
       <c r="G20" s="19">
+        <v>1</v>
+      </c>
+      <c r="H20" s="19">
         <v>2</v>
       </c>
-      <c r="H20" s="19">
+      <c r="I20" s="19">
+        <v>1</v>
+      </c>
+      <c r="K20" s="19">
+        <v>2</v>
+      </c>
+      <c r="L20" s="19">
         <v>100000</v>
       </c>
-      <c r="I20" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>3</v>
       </c>
@@ -2153,16 +2222,22 @@
         <v>1</v>
       </c>
       <c r="G21" s="19">
+        <v>1</v>
+      </c>
+      <c r="H21" s="19">
         <v>3</v>
       </c>
-      <c r="H21" s="19">
+      <c r="I21" s="19">
+        <v>1</v>
+      </c>
+      <c r="K21" s="19">
+        <v>3</v>
+      </c>
+      <c r="L21" s="19">
         <v>50000</v>
       </c>
-      <c r="I21" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>4</v>
       </c>
@@ -2177,26 +2252,32 @@
         <v>1</v>
       </c>
       <c r="G22" s="19">
+        <v>1</v>
+      </c>
+      <c r="H22" s="19">
         <v>4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="I22" s="19">
+        <v>1</v>
+      </c>
+      <c r="K22" s="19">
+        <v>4</v>
+      </c>
+      <c r="L22" s="19">
         <v>20000</v>
       </c>
-      <c r="I22" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>68</v>
       </c>
@@ -2211,7 +2292,7 @@
       <c r="F26" s="24"/>
       <c r="G26" s="23"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>1</v>
       </c>
@@ -2226,138 +2307,114 @@
       <c r="F27" s="24"/>
       <c r="G27" s="23"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="19">
+        <v>1</v>
+      </c>
+      <c r="B31" s="19">
+        <v>1</v>
+      </c>
+      <c r="C31" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
+        <v>2</v>
+      </c>
+      <c r="B32" s="19">
+        <v>1</v>
+      </c>
+      <c r="C32" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="19">
+        <v>3</v>
+      </c>
+      <c r="B33" s="19">
+        <v>1</v>
+      </c>
+      <c r="C33" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>4</v>
+      </c>
+      <c r="B34" s="19">
+        <v>1</v>
+      </c>
+      <c r="C34" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
-        <v>1</v>
-      </c>
-      <c r="B31" s="19">
-        <v>1</v>
-      </c>
-      <c r="C31" s="19">
-        <v>1</v>
-      </c>
-      <c r="D31" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
-        <v>1</v>
-      </c>
-      <c r="B32" s="19">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="19">
+        <v>1</v>
+      </c>
+      <c r="B38" s="19">
+        <v>1</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1</v>
+      </c>
+      <c r="D38" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>1</v>
+      </c>
+      <c r="B39" s="19">
+        <v>1</v>
+      </c>
+      <c r="C39" s="19">
         <v>2</v>
-      </c>
-      <c r="C32" s="19">
-        <v>1</v>
-      </c>
-      <c r="D32" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
-        <v>1</v>
-      </c>
-      <c r="B33" s="19">
-        <v>3</v>
-      </c>
-      <c r="C33" s="19">
-        <v>1</v>
-      </c>
-      <c r="D33" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
-        <v>1</v>
-      </c>
-      <c r="B34" s="19">
-        <v>4</v>
-      </c>
-      <c r="C34" s="19">
-        <v>1</v>
-      </c>
-      <c r="D34" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
-        <v>1</v>
-      </c>
-      <c r="B38" s="19">
-        <v>1</v>
-      </c>
-      <c r="C38" s="19">
-        <v>1</v>
-      </c>
-      <c r="D38" s="19">
-        <v>1</v>
-      </c>
-      <c r="E38" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
-        <v>1</v>
-      </c>
-      <c r="B39" s="19">
-        <v>1</v>
-      </c>
-      <c r="C39" s="19">
-        <v>1</v>
       </c>
       <c r="D39" s="19">
         <v>2</v>
       </c>
-      <c r="E39" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>1</v>
       </c>
@@ -2365,16 +2422,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D40" s="19">
         <v>3</v>
       </c>
-      <c r="E40" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>1</v>
       </c>
@@ -2382,65 +2436,56 @@
         <v>1</v>
       </c>
       <c r="C41" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D41" s="19">
         <v>4</v>
       </c>
-      <c r="E41" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="H44" s="35" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="L44" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="M44" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="N44" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>1</v>
       </c>
@@ -2451,28 +2496,34 @@
         <v>0</v>
       </c>
       <c r="D45" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E45" s="19">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="F45" s="19">
-        <v>2</v>
+        <v>900000</v>
       </c>
       <c r="G45" s="19">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H45" s="19">
-        <v>900000</v>
-      </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I45" s="19">
+        <v>0</v>
+      </c>
+      <c r="J45" s="19">
+        <v>0</v>
+      </c>
+      <c r="K45" s="19">
+        <v>0</v>
+      </c>
+      <c r="L45" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>2</v>
       </c>
@@ -2483,28 +2534,34 @@
         <v>0</v>
       </c>
       <c r="D46" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E46" s="19">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="F46" s="19">
-        <v>2</v>
+        <v>90000</v>
       </c>
       <c r="G46" s="19">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H46" s="19">
-        <v>90000</v>
-      </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I46" s="19">
+        <v>0</v>
+      </c>
+      <c r="J46" s="19">
+        <v>0</v>
+      </c>
+      <c r="K46" s="19">
+        <v>0</v>
+      </c>
+      <c r="L46" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>3</v>
       </c>
@@ -2515,28 +2572,34 @@
         <v>0</v>
       </c>
       <c r="D47" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E47" s="19">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F47" s="19">
-        <v>2</v>
+        <v>45000</v>
       </c>
       <c r="G47" s="19">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="H47" s="19">
-        <v>45000</v>
-      </c>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I47" s="19">
+        <v>0</v>
+      </c>
+      <c r="J47" s="19">
+        <v>0</v>
+      </c>
+      <c r="K47" s="19">
+        <v>0</v>
+      </c>
+      <c r="L47" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>4</v>
       </c>
@@ -2547,26 +2610,32 @@
         <v>0</v>
       </c>
       <c r="D48" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E48" s="19">
         <v>0</v>
       </c>
       <c r="F48" s="19">
-        <v>2</v>
+        <v>18000</v>
       </c>
       <c r="G48" s="19">
         <v>0</v>
       </c>
       <c r="H48" s="19">
-        <v>18000</v>
-      </c>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="19">
+        <v>0</v>
+      </c>
+      <c r="J48" s="19">
+        <v>0</v>
+      </c>
+      <c r="K48" s="19">
+        <v>0</v>
+      </c>
+      <c r="L48" s="19">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>